<commit_message>
File Uploaded Done Validation and toastr
</commit_message>
<xml_diff>
--- a/WebApp/wwwroot/uploads/Customers.xlsx
+++ b/WebApp/wwwroot/uploads/Customers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Review Management System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Venom\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE759C0E-6E49-45A5-A258-D39739CE86E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8A160E-8278-4C03-A1A1-7ABCB215366A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="11">
   <si>
     <t>FirstName</t>
   </si>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,7 +445,7 @@
       </c>
       <c r="E2" s="1">
         <f ca="1">TODAY()</f>
-        <v>45083</v>
+        <v>45084</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -463,14 +463,1345 @@
       </c>
       <c r="E3" s="1">
         <f ca="1">TODAY()</f>
-        <v>45083</v>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="1">
+        <v>45263</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="1">
+        <v>45265</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="1">
+        <f ca="1">TODAY()</f>
+        <v>45084</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{FEA7D50F-97AC-4A24-BC5D-59FF0250ACD3}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{41B03B1E-809C-4155-8D3A-E69884903768}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{257D8E4C-A06B-43E8-B6FC-E4DB7425F5A6}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{48BA85FC-56CC-41B4-8A18-DB0EF47B3A55}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{1ABDDA8D-B62E-491E-8ADA-6028914CE9AD}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{A65AC327-9E8B-4576-9C8F-8B2150B09F05}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{E4E4EA96-AD66-4907-A30B-B15420786232}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{B25694F7-E8B7-4176-A892-A5287209093E}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{647E9CE9-4863-4A6F-A459-5F4E9799FC1F}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{8230FBCB-6EF1-4F00-A8A4-F4CD1DCD7BB7}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{005C6E49-3722-4D22-8E7E-1D79B59C4CCA}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{4D592E90-2BF9-42D7-87D4-15C0650047F3}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{7C826BF8-63CD-4D83-8D28-C8AD3AAF76FF}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{FA5CE6C4-9179-4E89-B606-71C55F8C189A}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{DCFF47D0-5A6D-43BD-96EF-23E9EE8A3F38}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{13B9A459-F2D4-42F8-B996-6ED1264372E0}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{1AC0B016-FF62-40C1-A364-C1C48D8B0812}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{AE82325F-EB8D-4B22-99C8-7C8B20EADD6B}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{838C1223-AAFD-49E9-8FBE-5F2E0423DE7F}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{FB081C4E-2E2D-4D0A-8063-454E7F0C5D30}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{93FF10D3-707D-4BEF-B7CB-F2F1671043A0}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{4212CE08-5534-4EEF-A85A-86CD6D84E595}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{FE013890-E21E-43A3-A716-06EF57D3D74E}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{E1B74692-6B48-4CA4-B5B7-6CA20AF3FB3C}"/>
+    <hyperlink ref="D26" r:id="rId25" xr:uid="{A405BB84-442D-4C9B-9F4A-AFCA8475E9B5}"/>
+    <hyperlink ref="D27" r:id="rId26" xr:uid="{613025F5-17FE-4A94-901A-1505F1CE1F0B}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{E5080894-6729-4C04-A650-60FD2CAAFC44}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{F7D6D00B-BD8C-47ED-B439-8A5B42491684}"/>
+    <hyperlink ref="D30" r:id="rId29" xr:uid="{E29D02B7-F9F0-4DBA-A3CB-921138A6189A}"/>
+    <hyperlink ref="D31" r:id="rId30" xr:uid="{2164E2CE-687C-4AEA-BE8F-84ADE919F892}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{BDCEE500-05DD-4E44-9A44-D74001BF6118}"/>
+    <hyperlink ref="D33" r:id="rId32" xr:uid="{E412E63A-F94A-463A-AC45-0CC236EBE087}"/>
+    <hyperlink ref="D34" r:id="rId33" xr:uid="{43F2524F-2733-4515-AC51-5F4399B9E0FE}"/>
+    <hyperlink ref="D35" r:id="rId34" xr:uid="{98F8BA68-5773-4956-9437-BE8E38C9E83E}"/>
+    <hyperlink ref="D36" r:id="rId35" xr:uid="{77A260C7-5079-4D75-8C34-6962F680BBDE}"/>
+    <hyperlink ref="D37" r:id="rId36" xr:uid="{80220504-7843-45CE-BC0E-7B12351E6227}"/>
+    <hyperlink ref="D38" r:id="rId37" xr:uid="{2D36984C-5569-4AC2-8D63-64505EFFF416}"/>
+    <hyperlink ref="D39" r:id="rId38" xr:uid="{9DB6154E-7A03-4F5F-BB2E-65B8E1402FB7}"/>
+    <hyperlink ref="D40" r:id="rId39" xr:uid="{4DDE39A3-63B3-4689-B3A6-79B6B6BBD15A}"/>
+    <hyperlink ref="D41" r:id="rId40" xr:uid="{ED078226-7D8D-4950-8B4B-FE1A9483A29D}"/>
+    <hyperlink ref="D42" r:id="rId41" xr:uid="{2F0239B3-E5DF-44B9-94D1-321090E2F2DC}"/>
+    <hyperlink ref="D43" r:id="rId42" xr:uid="{1F123CCD-46A1-4A1F-9BE4-A68B6F99C4BF}"/>
+    <hyperlink ref="D44" r:id="rId43" xr:uid="{1DC9012A-9DE0-4B92-BB2D-7B670BF09E36}"/>
+    <hyperlink ref="D45" r:id="rId44" xr:uid="{BED39B5E-F03D-4070-8C82-183127E7FBEC}"/>
+    <hyperlink ref="D46" r:id="rId45" xr:uid="{F90C29D7-BFB6-4B20-B85A-64C729D7AD94}"/>
+    <hyperlink ref="D47" r:id="rId46" xr:uid="{5AB515E5-53D3-48DC-8C17-C22C3A4FA652}"/>
+    <hyperlink ref="D48" r:id="rId47" xr:uid="{9F4D9A46-3415-4EA3-B5B7-390788784E4E}"/>
+    <hyperlink ref="D49" r:id="rId48" xr:uid="{C9E7E886-E8E5-4B27-B595-98A1675A77B1}"/>
+    <hyperlink ref="D50" r:id="rId49" xr:uid="{8B91F05E-E36D-46BB-A2B3-BE16E8F40F0C}"/>
+    <hyperlink ref="D51" r:id="rId50" xr:uid="{97CD062C-61AB-4173-ADF1-81EA6C717F5F}"/>
+    <hyperlink ref="D52" r:id="rId51" xr:uid="{1B8D4E12-6952-41D3-B9F0-8B7F08476B19}"/>
+    <hyperlink ref="D53" r:id="rId52" xr:uid="{7D077BB3-928C-4F45-9772-6C3E60338357}"/>
+    <hyperlink ref="D54" r:id="rId53" xr:uid="{AFBE61E4-27DA-4976-AC3A-8CA6AAA2B1C3}"/>
+    <hyperlink ref="D55" r:id="rId54" xr:uid="{8B3360CB-1E47-4B8B-B54D-428B7880DE18}"/>
+    <hyperlink ref="D56" r:id="rId55" xr:uid="{B04316C0-57E1-48CC-8BB6-8002178573D6}"/>
+    <hyperlink ref="D57" r:id="rId56" xr:uid="{4E727EF3-511C-4475-B6CB-C7882D05ED3F}"/>
+    <hyperlink ref="D58" r:id="rId57" xr:uid="{B823C4BA-66AA-4643-B4E9-79FE18EC3268}"/>
+    <hyperlink ref="D59" r:id="rId58" xr:uid="{872AF29B-FB2A-4E70-9A01-39B966B28895}"/>
+    <hyperlink ref="D60" r:id="rId59" xr:uid="{3AD22BD5-A0C5-40A0-AFFA-676C9138760D}"/>
+    <hyperlink ref="D61" r:id="rId60" xr:uid="{F762EF04-74AA-46B9-B511-2FE5B9F6038D}"/>
+    <hyperlink ref="D62" r:id="rId61" xr:uid="{9737D1F6-0A5D-44E8-9E52-4FBEFB134D9E}"/>
+    <hyperlink ref="D63" r:id="rId62" xr:uid="{24949575-C6F4-49CB-A392-C64EE1DCBB95}"/>
+    <hyperlink ref="D64" r:id="rId63" xr:uid="{6B277444-B2C2-4BDD-8EAA-5EED1E5C4B54}"/>
+    <hyperlink ref="D65" r:id="rId64" xr:uid="{D363C82F-9F25-461C-86D3-86051F884F9C}"/>
+    <hyperlink ref="D66" r:id="rId65" xr:uid="{52CE3702-391C-4A24-91F9-2B90A81065D6}"/>
+    <hyperlink ref="D67" r:id="rId66" xr:uid="{0123A94E-1F4A-4632-B590-094E1FD61B54}"/>
+    <hyperlink ref="D68" r:id="rId67" xr:uid="{B9FC4235-B717-4E50-974E-59183564BADC}"/>
+    <hyperlink ref="D69" r:id="rId68" xr:uid="{F11C2E78-703B-4032-A0AA-264B65B3FD20}"/>
+    <hyperlink ref="D70" r:id="rId69" xr:uid="{F272D725-DC4C-4E15-B67E-9EC27B7F55DC}"/>
+    <hyperlink ref="D71" r:id="rId70" xr:uid="{1EC0FE40-9E65-46F0-80F2-35A070656E0F}"/>
+    <hyperlink ref="D72" r:id="rId71" xr:uid="{296E768E-80B2-4EE9-A07D-A23FD197D49E}"/>
+    <hyperlink ref="D73" r:id="rId72" xr:uid="{B89DE3D1-BFA0-41D8-9F29-120322099B24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
</xml_diff>